<commit_message>
add test data in test excel file
</commit_message>
<xml_diff>
--- a/src/com/cleartrip/testdata/ClearTripTestData.xlsx
+++ b/src/com/cleartrip/testdata/ClearTripTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Browser</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Hellos</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,6 +450,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>